<commit_message>
Added robots, sitemap and recaptcha
</commit_message>
<xml_diff>
--- a/docker/content.xlsx
+++ b/docker/content.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="languages" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="portfolio" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="content" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="projects" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="languages" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="portfolio" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="content" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="projects" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="146">
   <si>
     <t xml:space="preserve">language</t>
   </si>
@@ -193,97 +193,96 @@
     <t xml:space="preserve">error_subtitle</t>
   </si>
   <si>
-    <t xml:space="preserve">We have taken note of the error and will try to fix it as soon as possible.</t>
+    <t xml:space="preserve">This is strange, but I couldn't catch where you wanted to go. 
+Please, return to home and use the available options.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">404_error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">404 Page Not Found!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inicio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sobre mí</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proyectos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contacto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestionar Contenido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Editar Inicio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Editar Sobre Mí</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Editar Proyectos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Editar Contacto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cerrar Sesión</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ponte en contacto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sígueme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inicio Sesión</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre de Usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contraseña</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recuérdame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre de Usuario o Contraseña no válidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leer más</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palabras clave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anterior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siguiente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lectura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Escribe y pulsa Enter para buscar projectos…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buscar palabras clave…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algo ha ido mal.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esto es extraño, pero no pude entender a dónde querías ir. 
+Por favor, vuelve a la página principal y usa las opciones disponibles.</t>
   </si>
   <si>
     <t xml:space="preserve">back_home</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Back To Home</t>
-  </si>
-  <si>
-    <t xml:space="preserve">404_error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">404 Page Not Found!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inicio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sobre mí</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proyectos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contacto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestionar Contenido</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Editar Inicio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Editar Sobre Mí</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Editar Proyectos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Editar Contacto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cerrar Sesión</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ponte en contacto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sígueme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inicio Sesión</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre de Usuario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contraseña</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recuérdame</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre de Usuario o Contraseña no válidos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leer más</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Palabras clave</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anterior</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Siguiente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lectura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Escribe y pulsa Enter para buscar projectos…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buscar palabras clave…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Algo ha ido mal.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hemos tomado nota del error, lo intentaremos solucionar lo antes posible.</t>
   </si>
   <si>
     <t xml:space="preserve">Volver A Inicio</t>
@@ -574,7 +573,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -599,6 +598,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -620,7 +623,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -635,14 +638,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,6 +650,112 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -665,7 +766,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="1" sqref="54:56 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -706,10 +807,10 @@
   </sheetPr>
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D53" activeCellId="0" sqref="D53"/>
+      <selection pane="bottomLeft" activeCell="A54" activeCellId="0" sqref="54:56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -998,48 +1099,51 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="1" t="s">
+    <row r="26" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="1" t="s">
+    <row r="27" s="6" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" s="5" t="s">
+      <c r="C27" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="1" t="s">
+    <row r="28" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>60</v>
+      <c r="D29" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1049,8 +1153,8 @@
       <c r="C30" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>61</v>
+      <c r="D30" s="8" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1061,7 +1165,7 @@
         <v>2</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1072,7 +1176,7 @@
         <v>2</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1083,7 +1187,7 @@
         <v>2</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1094,7 +1198,7 @@
         <v>2</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1105,7 +1209,7 @@
         <v>2</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1116,7 +1220,7 @@
         <v>2</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1127,7 +1231,7 @@
         <v>2</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1138,7 +1242,7 @@
         <v>2</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1149,7 +1253,7 @@
         <v>2</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1160,7 +1264,7 @@
         <v>2</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1171,7 +1275,7 @@
         <v>2</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1182,7 +1286,7 @@
         <v>2</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1193,7 +1297,7 @@
         <v>2</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1204,7 +1308,7 @@
         <v>2</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1215,7 +1319,7 @@
         <v>2</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1226,7 +1330,7 @@
         <v>2</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1237,7 +1341,7 @@
         <v>2</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1248,7 +1352,7 @@
         <v>2</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1259,7 +1363,7 @@
         <v>2</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1270,7 +1374,7 @@
         <v>2</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1280,11 +1384,11 @@
       <c r="C51" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D51" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="52" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D51" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5"/>
       <c r="B52" s="5" t="s">
         <v>49</v>
@@ -1293,10 +1397,10 @@
         <v>2</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="53" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5"/>
       <c r="B53" s="5" t="s">
         <v>51</v>
@@ -1305,10 +1409,10 @@
         <v>2</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="54" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5"/>
       <c r="B54" s="5" t="s">
         <v>53</v>
@@ -1317,43 +1421,42 @@
         <v>2</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="55" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="56" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C55" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5"/>
       <c r="B56" s="5" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="57" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="57" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5"/>
       <c r="B57" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D57" s="6" t="s">
-        <v>88</v>
+      <c r="D57" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1377,7 +1480,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D39" activeCellId="0" sqref="D39"/>
+      <selection pane="bottomLeft" activeCell="D39" activeCellId="1" sqref="54:56 D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1387,7 +1490,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="124.9"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1403,24 +1506,24 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>90</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
@@ -1428,36 +1531,36 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="11"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>94</v>
+      <c r="D5" s="11" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
@@ -1465,94 +1568,94 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="10"/>
+      <c r="D8" s="11"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="11"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="10"/>
-    </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="11"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="10"/>
-    </row>
-    <row r="11" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="11"/>
-    </row>
-    <row r="12" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="11"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="10"/>
-    </row>
-    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="C13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="10"/>
+      <c r="D13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>1</v>
@@ -1560,144 +1663,144 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>102</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="10"/>
+      <c r="D16" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="10"/>
+      <c r="D17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="10"/>
+      <c r="D18" s="11"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="11"/>
+      <c r="D19" s="12"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="10"/>
+      <c r="D20" s="11"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="11"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="10"/>
-    </row>
-    <row r="22" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="11"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="10"/>
-    </row>
-    <row r="23" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="11"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="10"/>
-    </row>
-    <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="11"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="10"/>
-    </row>
-    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="C25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="10"/>
+      <c r="D25" s="11"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>2</v>
@@ -1705,285 +1808,285 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="10" t="s">
-        <v>108</v>
+      <c r="D27" s="11" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="10"/>
+      <c r="D28" s="11"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="10"/>
+      <c r="D29" s="11"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="10"/>
+      <c r="D30" s="11"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="11"/>
+      <c r="D31" s="12"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D33" s="10" t="s">
-        <v>112</v>
+      <c r="D33" s="11" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="11" t="s">
         <v>115</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="11" t="s">
         <v>117</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="11" t="s">
         <v>119</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="11" t="s">
         <v>121</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D39" s="10"/>
+      <c r="D39" s="11"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="C40" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="D40" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="11" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="10" t="s">
-        <v>126</v>
+      <c r="D42" s="11" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="10" t="s">
-        <v>127</v>
+      <c r="D43" s="11" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D44" s="10" t="s">
-        <v>128</v>
+      <c r="D44" s="11" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D45" s="10" t="s">
-        <v>129</v>
+      <c r="D45" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D46" s="10" t="s">
-        <v>130</v>
+      <c r="D46" s="11" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D47" s="10"/>
+      <c r="D47" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2003,15 +2106,15 @@
   </sheetPr>
   <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="1" sqref="54:56 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="12" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="13" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="28.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="24.66"/>
@@ -2022,60 +2125,60 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="24" min="10" style="1" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+    <row r="1" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>131</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>132</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
@@ -2085,23 +2188,23 @@
       <c r="X1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13"/>
+      <c r="A2" s="14"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="14"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="15"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13"/>
+      <c r="A3" s="14"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="14"/>
+      <c r="H3" s="15"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13"/>
+      <c r="A4" s="14"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="15"/>
@@ -2109,8 +2212,8 @@
       <c r="P4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13"/>
-      <c r="B5" s="8"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="9"/>
       <c r="F5" s="4"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
@@ -2118,7 +2221,7 @@
       <c r="P5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13"/>
+      <c r="A6" s="14"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="15"/>
@@ -2127,7 +2230,7 @@
       <c r="P6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13"/>
+      <c r="A7" s="14"/>
       <c r="F7" s="4"/>
       <c r="G7" s="15"/>
       <c r="H7" s="4"/>
@@ -2136,8 +2239,8 @@
       <c r="P7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13"/>
-      <c r="F8" s="16"/>
+      <c r="A8" s="14"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="O8" s="5"/>
@@ -2146,7 +2249,7 @@
       <c r="R8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13"/>
+      <c r="A9" s="14"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>

</xml_diff>